<commit_message>
Maschien Vision approach to segemntation task
</commit_message>
<xml_diff>
--- a/Expert_Analysis.xlsx
+++ b/Expert_Analysis.xlsx
@@ -511,7 +511,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -639,7 +639,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -735,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1007,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1167,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1295,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1343,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1359,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="C58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1375,7 +1375,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1391,7 +1391,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="C61" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         <v>3</v>
       </c>
       <c r="C63" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1455,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="C64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1535,7 +1535,7 @@
         <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1839,7 +1839,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -1871,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -1903,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -1919,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -1999,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="C98" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2255,7 +2255,7 @@
         <v>4</v>
       </c>
       <c r="C114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
         <v>3</v>
       </c>
       <c r="C116" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -2447,7 +2447,7 @@
         <v>3</v>
       </c>
       <c r="C126" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -2575,7 +2575,7 @@
         <v>3</v>
       </c>
       <c r="C134" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -2591,7 +2591,7 @@
         <v>3</v>
       </c>
       <c r="C135" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -2719,7 +2719,7 @@
         <v>4</v>
       </c>
       <c r="C143" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -2735,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="C144" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -2767,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="C146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -2815,7 +2815,7 @@
         <v>3</v>
       </c>
       <c r="C149" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="C152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -2975,7 +2975,7 @@
         <v>3</v>
       </c>
       <c r="C159" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -3007,7 +3007,7 @@
         <v>2</v>
       </c>
       <c r="C161" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -3055,7 +3055,7 @@
         <v>3</v>
       </c>
       <c r="C164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>

</xml_diff>